<commit_message>
Adding program links to dashboard
</commit_message>
<xml_diff>
--- a/data/DPO_app_intervention_names.xlsx
+++ b/data/DPO_app_intervention_names.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoregon-my.sharepoint.com/personal/strevino_uoregon_edu/Documents/Desktop/HEDCO Institute/GitHub R Projects/Depression_Prevention_Overview/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{8A08B8BF-4197-4250-9F47-B55103264D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{396A5D19-3F61-4F53-ABFA-E7C11D936DCC}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="8_{8A08B8BF-4197-4250-9F47-B55103264D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17566173-E6ED-43FB-8978-4891535000E9}"/>
   <bookViews>
-    <workbookView xWindow="-16356" yWindow="348" windowWidth="16224" windowHeight="13092" activeTab="2" xr2:uid="{ECE45DD1-0422-437C-B3F3-CDDA7BE602A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{ECE45DD1-0422-437C-B3F3-CDDA7BE602A8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Links" sheetId="3" r:id="rId1"/>
-    <sheet name="Rename" sheetId="1" r:id="rId2"/>
-    <sheet name="Definitions" sheetId="2" r:id="rId3"/>
+    <sheet name="Rename" sheetId="1" r:id="rId1"/>
+    <sheet name="Definitions" sheetId="2" r:id="rId2"/>
+    <sheet name="Links" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Links!$A$1:$C$65</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Rename!$C$1:$F$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Links!$A$1:$D$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Rename!$C$1:$F$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="236">
   <si>
     <t>Intervention</t>
   </si>
@@ -605,12 +605,6 @@
     <t>Aussie Optimism</t>
   </si>
   <si>
-    <t xml:space="preserve">Aussie Optimism Program: </t>
-  </si>
-  <si>
-    <t>Feelings and Friends (AOP-FF)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cognitive-behavior program (CB); </t>
   </si>
   <si>
@@ -636,13 +630,136 @@
   </si>
   <si>
     <t>clearinghouse_link</t>
+  </si>
+  <si>
+    <t>group_number</t>
+  </si>
+  <si>
+    <t>https://trove.nla.gov.au/work/26289193</t>
+  </si>
+  <si>
+    <t>https://www.saavsus.com/adolescent-coping-with-depression-course</t>
+  </si>
+  <si>
+    <t>https://www.cebc4cw.org/program/adolescent-coping-with-depression-course-cwd-a/detailed</t>
+  </si>
+  <si>
+    <t>https://sites.pitt.edu/~krp12/</t>
+  </si>
+  <si>
+    <t>https://www.cebc4cw.org/program/teaching-kids-to-cope-tkc/#:~:text=Teaching%20Kids%20to%20Cope%20%28TKC%29%201%20About%20This,Training%20...%205%20Relevant%20Published%2C%20Peer-Reviewed%20Research%20</t>
+  </si>
+  <si>
+    <t>https://ppc.sas.upenn.edu/services/penn-resilience-training</t>
+  </si>
+  <si>
+    <t>https://www.euda.europa.eu/best-practice/xchange/penn-resiliency-programme-prp-op-volle-kracht-full-power-netherlands-uk-resiliency-programme-uk-school-based-group-intervention-teaching-cognitive-behavioural-and-social-problem-solving-skills_en</t>
+  </si>
+  <si>
+    <t>https://www.sparx.org.nz/</t>
+  </si>
+  <si>
+    <t>https://www.c4tbh.org/program-review/smart-positive-active-realistic-x-factor-thoughts-sparx/</t>
+  </si>
+  <si>
+    <t>https://thiswayup.org.au/</t>
+  </si>
+  <si>
+    <t>https://www.rap.qut.edu.au/</t>
+  </si>
+  <si>
+    <t>https://www.cebc4cw.org/program/resourceful-adolescent-program-adolescent-rap-a/</t>
+  </si>
+  <si>
+    <t>https://www.beyondblue.org.au/</t>
+  </si>
+  <si>
+    <t>https://aussieoptimism.com.au/</t>
+  </si>
+  <si>
+    <t>https://positivechoices.org.au/teachers/aussie-optimism-program</t>
+  </si>
+  <si>
+    <t>https://www.amazon.de/Trainingsprogramm-Pr%C3%A4vention-Depressionen-Jugendlichen-Therapeutische/dp/380171800X</t>
+  </si>
+  <si>
+    <t>https://mindfulnessinschools.org/</t>
+  </si>
+  <si>
+    <t>https://pg.casel.org/b/</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/book/1241/chapter-abstract/140165435?redirectedFrom=fulltext</t>
+  </si>
+  <si>
+    <t>https://www.cebc4cw.org/program/interpersonal-psychotherapy-adolescent-skills-training/detailed</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/10.1002/9781118269848.ch4</t>
+  </si>
+  <si>
+    <t>https://www.moodgym.com.au/</t>
+  </si>
+  <si>
+    <t>https://cdc.thehcn.net/promisepractice/index/view?pid=3835</t>
+  </si>
+  <si>
+    <t>https://explore.bps.org.uk/content/bpstcp/5/2/90</t>
+  </si>
+  <si>
+    <t>https://depression.hku.hk/en/the-storm/</t>
+  </si>
+  <si>
+    <t>https://www.rap.qut.edu.au/programs/rap-p-for-parents</t>
+  </si>
+  <si>
+    <t>https://www.themhs.org/resource/adolescents-coping-with-emotions-ace-program/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Learned-Optimism-Change-Your-Mind/dp/1400078393</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Transdiagnostic-Treatment-Emotional-Disorders-Adolescents/dp/0190855533</t>
+  </si>
+  <si>
+    <t>https://slam.nhs.uk/discover/</t>
+  </si>
+  <si>
+    <t>https://www.workbookpublishing.com/group-leader-manual-for-emotion-coping-kids-managing-anxiety-and-depression.html</t>
+  </si>
+  <si>
+    <t>https://www.cebc4cw.org/program/emotion-coping-kids-managing-anxiety-and-depression/</t>
+  </si>
+  <si>
+    <t>https://www.blueprintsprograms.org/programs/596999999/adolescent-coping-with-depression/</t>
+  </si>
+  <si>
+    <t>https://aussieoptimism.com.au/programs/positive-thinking/</t>
+  </si>
+  <si>
+    <t>The Optimism and Life Skills Program (adapted from Penn Depression Prevention Program)</t>
+  </si>
+  <si>
+    <t>Cognitive-behavior program (CB; adapted); interpersonal psychotherapy–adolescent skills training (IPT-AST)</t>
+  </si>
+  <si>
+    <t>https://research.kpchr.org/Research/Research-Areas/Mental-Health/Youth-Depression-Programs#Downloads</t>
+  </si>
+  <si>
+    <t>http://www.mentalhealthpromotion.net/?i=promenpol.en.toolkit.343</t>
+  </si>
+  <si>
+    <t>UK Resilience Programme (UKRP) - adapted from Penn Resiliency Program</t>
+  </si>
+  <si>
+    <t>https://guidebook.eif.org.uk/programme/penn-resilience-programme-uk-implementation-in-primary-school</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -657,13 +774,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -675,17 +806,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1025,761 +1179,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504B7D24-44EE-4748-B674-AFAEE10AE69B}">
-  <dimension ref="A1:E65"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="86" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>31883</v>
-      </c>
-      <c r="B2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>31881</v>
-      </c>
-      <c r="B3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>31881</v>
-      </c>
-      <c r="B4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>31835</v>
-      </c>
-      <c r="B5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>32054</v>
-      </c>
-      <c r="B6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>31815</v>
-      </c>
-      <c r="B7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>31953</v>
-      </c>
-      <c r="B8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>31857</v>
-      </c>
-      <c r="B9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>31857</v>
-      </c>
-      <c r="B10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>31882</v>
-      </c>
-      <c r="B11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>31858</v>
-      </c>
-      <c r="B12" t="s">
-        <v>135</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>31868</v>
-      </c>
-      <c r="B13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>31868</v>
-      </c>
-      <c r="B14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>31853</v>
-      </c>
-      <c r="B15" t="s">
-        <v>136</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>31885</v>
-      </c>
-      <c r="B16" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>31885</v>
-      </c>
-      <c r="B17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>32232</v>
-      </c>
-      <c r="B18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>31792</v>
-      </c>
-      <c r="B19" t="s">
-        <v>156</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>31909</v>
-      </c>
-      <c r="B20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>32180</v>
-      </c>
-      <c r="B21" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>32283</v>
-      </c>
-      <c r="B22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>31886</v>
-      </c>
-      <c r="B23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>31915</v>
-      </c>
-      <c r="B24" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>32203</v>
-      </c>
-      <c r="B25" t="s">
-        <v>110</v>
-      </c>
-      <c r="C25" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>31788</v>
-      </c>
-      <c r="B26" t="s">
-        <v>133</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>31920</v>
-      </c>
-      <c r="B27" t="s">
-        <v>167</v>
-      </c>
-      <c r="C27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>31863</v>
-      </c>
-      <c r="B28" t="s">
-        <v>168</v>
-      </c>
-      <c r="C28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>31958</v>
-      </c>
-      <c r="B29" t="s">
-        <v>160</v>
-      </c>
-      <c r="C29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>31867</v>
-      </c>
-      <c r="B30" t="s">
-        <v>150</v>
-      </c>
-      <c r="C30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>31904</v>
-      </c>
-      <c r="B31" t="s">
-        <v>138</v>
-      </c>
-      <c r="C31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>32269</v>
-      </c>
-      <c r="B32" t="s">
-        <v>145</v>
-      </c>
-      <c r="C32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32265</v>
-      </c>
-      <c r="B33" t="s">
-        <v>140</v>
-      </c>
-      <c r="C33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>31845</v>
-      </c>
-      <c r="B34" t="s">
-        <v>114</v>
-      </c>
-      <c r="C34" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>31879</v>
-      </c>
-      <c r="B35" t="s">
-        <v>119</v>
-      </c>
-      <c r="C35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>31809</v>
-      </c>
-      <c r="B36" t="s">
-        <v>113</v>
-      </c>
-      <c r="C36" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>31809</v>
-      </c>
-      <c r="B37" t="s">
-        <v>113</v>
-      </c>
-      <c r="C37" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>31809</v>
-      </c>
-      <c r="B38" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>31870</v>
-      </c>
-      <c r="B39" t="s">
-        <v>157</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>31859</v>
-      </c>
-      <c r="B40" t="s">
-        <v>153</v>
-      </c>
-      <c r="C40" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>31901</v>
-      </c>
-      <c r="B41" t="s">
-        <v>141</v>
-      </c>
-      <c r="C41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>32316</v>
-      </c>
-      <c r="B42" t="s">
-        <v>142</v>
-      </c>
-      <c r="C42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>31855</v>
-      </c>
-      <c r="B43" t="s">
-        <v>144</v>
-      </c>
-      <c r="C43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>31818</v>
-      </c>
-      <c r="B44" t="s">
-        <v>125</v>
-      </c>
-      <c r="C44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>31816</v>
-      </c>
-      <c r="B45" t="s">
-        <v>131</v>
-      </c>
-      <c r="C45" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>31848</v>
-      </c>
-      <c r="B46" t="s">
-        <v>155</v>
-      </c>
-      <c r="C46" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>31860</v>
-      </c>
-      <c r="B47" t="s">
-        <v>132</v>
-      </c>
-      <c r="C47" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>31950</v>
-      </c>
-      <c r="B48" t="s">
-        <v>159</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>31950</v>
-      </c>
-      <c r="B49" t="s">
-        <v>159</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>32238</v>
-      </c>
-      <c r="B50" t="s">
-        <v>139</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>32238</v>
-      </c>
-      <c r="B51" t="s">
-        <v>139</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>31851</v>
-      </c>
-      <c r="B52" t="s">
-        <v>121</v>
-      </c>
-      <c r="C52" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>32067</v>
-      </c>
-      <c r="B53" t="s">
-        <v>151</v>
-      </c>
-      <c r="C53" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>31847</v>
-      </c>
-      <c r="B54" t="s">
-        <v>128</v>
-      </c>
-      <c r="C54" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>32320</v>
-      </c>
-      <c r="B55" t="s">
-        <v>129</v>
-      </c>
-      <c r="C55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>32288</v>
-      </c>
-      <c r="B56" t="s">
-        <v>106</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>31875</v>
-      </c>
-      <c r="B57" t="s">
-        <v>149</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>31869</v>
-      </c>
-      <c r="B58" t="s">
-        <v>108</v>
-      </c>
-      <c r="C58" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>31807</v>
-      </c>
-      <c r="B59" t="s">
-        <v>152</v>
-      </c>
-      <c r="C59" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>31947</v>
-      </c>
-      <c r="B60" t="s">
-        <v>130</v>
-      </c>
-      <c r="C60" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>31865</v>
-      </c>
-      <c r="B61" t="s">
-        <v>158</v>
-      </c>
-      <c r="C61" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>31842</v>
-      </c>
-      <c r="B62" t="s">
-        <v>122</v>
-      </c>
-      <c r="C62" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>32233</v>
-      </c>
-      <c r="B63" t="s">
-        <v>115</v>
-      </c>
-      <c r="C63" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>32174</v>
-      </c>
-      <c r="B64" t="s">
-        <v>123</v>
-      </c>
-      <c r="C64" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>32137</v>
-      </c>
-      <c r="B65" t="s">
-        <v>166</v>
-      </c>
-      <c r="C65" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:C65" xr:uid="{504B7D24-44EE-4748-B674-AFAEE10AE69B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C65">
-      <sortCondition ref="C1:C65"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09150482-75BD-4133-A06F-6CE7E7EB8102}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2546,6 +1950,9 @@
       <c r="C41" t="s">
         <v>42</v>
       </c>
+      <c r="D41" t="s">
+        <v>231</v>
+      </c>
       <c r="E41" t="s">
         <v>66</v>
       </c>
@@ -2817,6 +2224,9 @@
       </c>
       <c r="C57" t="s">
         <v>56</v>
+      </c>
+      <c r="D57" t="s">
+        <v>230</v>
       </c>
       <c r="E57" t="s">
         <v>66</v>
@@ -3073,11 +2483,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ADF9C74-2290-4105-B3AB-9883F995AA4B}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3277,4 +2687,1337 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504B7D24-44EE-4748-B674-AFAEE10AE69B}">
+  <dimension ref="A1:F64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125"/>
+    <col min="4" max="4" width="86" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="52.7109375" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>31788</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>31792</v>
+      </c>
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>31807</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>31809</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>31809</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>31809</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>31815</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>31816</v>
+      </c>
+      <c r="B9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>31818</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>31835</v>
+      </c>
+      <c r="B11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>31842</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>31845</v>
+      </c>
+      <c r="B13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>31847</v>
+      </c>
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>31848</v>
+      </c>
+      <c r="B15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>31851</v>
+      </c>
+      <c r="B16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>31853</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>31855</v>
+      </c>
+      <c r="B18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>31857</v>
+      </c>
+      <c r="B19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>184</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>31857</v>
+      </c>
+      <c r="B20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>185</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>31858</v>
+      </c>
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>31859</v>
+      </c>
+      <c r="B22" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>31860</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>31863</v>
+      </c>
+      <c r="B24" t="s">
+        <v>168</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>31865</v>
+      </c>
+      <c r="B25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>31867</v>
+      </c>
+      <c r="B26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>31868</v>
+      </c>
+      <c r="B27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>31869</v>
+      </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>31870</v>
+      </c>
+      <c r="B29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>31875</v>
+      </c>
+      <c r="B30" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31879</v>
+      </c>
+      <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31881</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>182</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31881</v>
+      </c>
+      <c r="B33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>183</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31882</v>
+      </c>
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>31883</v>
+      </c>
+      <c r="B35" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>31885</v>
+      </c>
+      <c r="B36" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>186</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>31885</v>
+      </c>
+      <c r="B37" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>187</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>31886</v>
+      </c>
+      <c r="B38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>31901</v>
+      </c>
+      <c r="B39" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>31904</v>
+      </c>
+      <c r="B40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>31909</v>
+      </c>
+      <c r="B41" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>31915</v>
+      </c>
+      <c r="B42" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>31920</v>
+      </c>
+      <c r="B43" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>31947</v>
+      </c>
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>31950</v>
+      </c>
+      <c r="B45" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>31950</v>
+      </c>
+      <c r="B46" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>31953</v>
+      </c>
+      <c r="B47" t="s">
+        <v>148</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>31958</v>
+      </c>
+      <c r="B48" t="s">
+        <v>160</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>32054</v>
+      </c>
+      <c r="B49" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>32067</v>
+      </c>
+      <c r="B50" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>32137</v>
+      </c>
+      <c r="B51" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>32174</v>
+      </c>
+      <c r="B52" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>234</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>32180</v>
+      </c>
+      <c r="B53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>32203</v>
+      </c>
+      <c r="B54" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>32232</v>
+      </c>
+      <c r="B55" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>32233</v>
+      </c>
+      <c r="B56" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>32238</v>
+      </c>
+      <c r="B57" t="s">
+        <v>139</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>32238</v>
+      </c>
+      <c r="B58" t="s">
+        <v>139</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>32265</v>
+      </c>
+      <c r="B59" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>39</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>32269</v>
+      </c>
+      <c r="B60" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>39</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>32283</v>
+      </c>
+      <c r="B61" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>32288</v>
+      </c>
+      <c r="B62" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>32316</v>
+      </c>
+      <c r="B63" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>41</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>32320</v>
+      </c>
+      <c r="B64" t="s">
+        <v>129</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>71</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D65" xr:uid="{504B7D24-44EE-4748-B674-AFAEE10AE69B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D65">
+      <sortCondition ref="B1:B65"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
+    <sortCondition ref="A2:A64"/>
+  </sortState>
+  <conditionalFormatting sqref="B1:C1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="F45" r:id="rId1" xr:uid="{8378A75F-103E-494E-BCD6-7E8B0FC2607A}"/>
+    <hyperlink ref="F57" r:id="rId2" xr:uid="{1EF98329-AD6E-4032-A1E0-D712A8F13790}"/>
+    <hyperlink ref="F50" r:id="rId3" xr:uid="{17F69C15-BC09-4D1C-ACD2-30F2650F42D3}"/>
+    <hyperlink ref="F62" r:id="rId4" xr:uid="{BAFE6581-8387-44F8-9581-6056EF67AD2B}"/>
+    <hyperlink ref="F30" r:id="rId5" xr:uid="{4681AFB0-1100-4894-B106-BAB05E220DC9}"/>
+    <hyperlink ref="F23" r:id="rId6" xr:uid="{0E1741F3-B332-472E-93EE-30490FD72656}"/>
+    <hyperlink ref="F16" r:id="rId7" xr:uid="{B2BE18D4-8FFF-4DCA-A8E7-29C6070FDC14}"/>
+    <hyperlink ref="F14" r:id="rId8" xr:uid="{06DC273A-1AA0-49F3-96C2-1B38917EE67A}"/>
+    <hyperlink ref="F64" r:id="rId9" xr:uid="{071B8E4E-EF55-41B5-B9CA-5C50C5ED8A33}"/>
+    <hyperlink ref="F39" r:id="rId10" xr:uid="{ECE55C7D-5F7C-4CD6-AE7B-BB776B91FEC0}"/>
+    <hyperlink ref="F63" r:id="rId11" xr:uid="{F528B45E-8A70-4F2B-9B56-34EA1D177F91}"/>
+    <hyperlink ref="F29" r:id="rId12" xr:uid="{9F8E7070-E516-4E38-8727-D35DDAF3AAFA}"/>
+    <hyperlink ref="F5" r:id="rId13" xr:uid="{4C671029-11A2-42D4-90B6-FE8A2F496E66}"/>
+    <hyperlink ref="F34" r:id="rId14" xr:uid="{6E7B255F-A1E6-47AD-AF0E-0E0134578ACE}"/>
+    <hyperlink ref="F21" r:id="rId15" xr:uid="{AF042E5E-FAFF-454F-876A-99CC8A53F2D8}"/>
+    <hyperlink ref="F27" r:id="rId16" xr:uid="{5FCE0664-D7B0-41A6-90BA-460A778BBD4E}"/>
+    <hyperlink ref="F19" r:id="rId17" xr:uid="{E907D68D-C888-4FC2-A814-F8543EAE33BA}"/>
+    <hyperlink ref="F20" r:id="rId18" xr:uid="{0D2AFB46-6043-43B0-91B3-3016DD2F06D8}"/>
+    <hyperlink ref="E23" r:id="rId19" xr:uid="{F7EA67C3-4E5A-4E4A-BAC7-814EDDD6604F}"/>
+    <hyperlink ref="E45" r:id="rId20" xr:uid="{E211FF3E-8ACA-4D6F-9E5D-DFE9755EF792}"/>
+    <hyperlink ref="E57" r:id="rId21" xr:uid="{01A2681D-B4A1-4CA1-94E5-12FAEAB52794}"/>
+    <hyperlink ref="E16" r:id="rId22" xr:uid="{B0917317-6B73-48E2-8AC8-1820D1B7E9F0}"/>
+    <hyperlink ref="E50" r:id="rId23" xr:uid="{0188ED8A-3E1A-4320-BE5A-F1FC88B927CC}"/>
+    <hyperlink ref="E14" r:id="rId24" xr:uid="{5AD57216-123A-4604-BA8C-514093EC5656}"/>
+    <hyperlink ref="E64" r:id="rId25" xr:uid="{3A07E0DC-5F13-4DBB-B768-03A3683F2F2B}"/>
+    <hyperlink ref="E62" r:id="rId26" xr:uid="{D7BB18F4-8F0E-4144-A0EF-19C7CDD337CC}"/>
+    <hyperlink ref="E30" r:id="rId27" xr:uid="{113F81A6-9FBE-4EF0-BF55-D14AD78DC90F}"/>
+    <hyperlink ref="E29" r:id="rId28" xr:uid="{881201B8-A3DC-44FF-AF57-F959E27D70B4}"/>
+    <hyperlink ref="E22" r:id="rId29" xr:uid="{74D36768-F7E8-4844-99A6-F07AECA72B32}"/>
+    <hyperlink ref="E39" r:id="rId30" xr:uid="{A13FF7A5-9F91-4F1A-8B36-38D83EBA4CF6}"/>
+    <hyperlink ref="E63" r:id="rId31" xr:uid="{F832A250-EF1C-43A1-B152-5FAC9AD93157}"/>
+    <hyperlink ref="E13" r:id="rId32" xr:uid="{20AF2881-6D13-4C13-9979-EC975005CFB4}"/>
+    <hyperlink ref="E31" r:id="rId33" xr:uid="{0CB9A7E8-C383-4B63-ACAE-18F513DC04BA}"/>
+    <hyperlink ref="E5" r:id="rId34" xr:uid="{F1FFB753-1476-4A4E-85B6-FB513D590226}"/>
+    <hyperlink ref="E20" r:id="rId35" xr:uid="{E9771604-DF3A-43B7-A7DB-E53876A949F9}"/>
+    <hyperlink ref="E19" r:id="rId36" xr:uid="{4A162E7F-061C-4A0C-A88B-8FD04AB15516}"/>
+    <hyperlink ref="E34" r:id="rId37" xr:uid="{BA8288E1-5257-44C8-A76C-AD2147C98CA6}"/>
+    <hyperlink ref="E21" r:id="rId38" xr:uid="{8752A4AB-09BC-4D5E-8CF3-94D69B96AC52}"/>
+    <hyperlink ref="E27" r:id="rId39" xr:uid="{6620F9ED-DF56-402D-AB42-71003A0D8EA4}"/>
+    <hyperlink ref="E43" r:id="rId40" xr:uid="{5B949B19-D0A2-49FD-8D74-A9D7987E97A8}"/>
+    <hyperlink ref="E24" r:id="rId41" xr:uid="{DDDA1C3D-CB6F-4A49-8123-0F1377530EFC}"/>
+    <hyperlink ref="E26" r:id="rId42" xr:uid="{BF859DE6-C972-40AC-876E-6A05A58DEDB3}"/>
+    <hyperlink ref="E40" r:id="rId43" xr:uid="{859D5689-2AFC-47D9-9CDA-A1D5E95D534D}"/>
+    <hyperlink ref="E60" r:id="rId44" xr:uid="{DA936187-D053-4EA4-800E-AA1C70DFC567}"/>
+    <hyperlink ref="E59" r:id="rId45" xr:uid="{2B63FB07-176A-497B-B8A7-F76B009DC435}"/>
+    <hyperlink ref="F40" r:id="rId46" xr:uid="{66144401-076B-4D65-9B27-0F62CD92215C}"/>
+    <hyperlink ref="F60" r:id="rId47" xr:uid="{C9DB3F47-D825-4972-8C6F-6937F50DF437}"/>
+    <hyperlink ref="F59" r:id="rId48" xr:uid="{554860CA-220F-45D1-879B-A791B2E88D8C}"/>
+    <hyperlink ref="E35" r:id="rId49" xr:uid="{3F575516-1D65-4892-920A-97F6439B631E}"/>
+    <hyperlink ref="E33" r:id="rId50" xr:uid="{7A6C9AF8-5CCE-4A70-9BDF-A7383AA9FB4E}"/>
+    <hyperlink ref="E32" r:id="rId51" xr:uid="{744DE233-DC04-4235-907E-64E5F19A23BC}"/>
+    <hyperlink ref="F35" r:id="rId52" xr:uid="{B20D6884-6865-4E1E-9E88-247DF5EF294E}"/>
+    <hyperlink ref="F33" r:id="rId53" xr:uid="{3112B712-3917-4CB6-9414-FB164FC2940A}"/>
+    <hyperlink ref="F32" r:id="rId54" xr:uid="{AA037FD7-70D4-42E3-9D2E-AC7BC4A77AE1}"/>
+    <hyperlink ref="E49" r:id="rId55" xr:uid="{E4FA4305-BC77-40FB-9B4C-0AE98E9FE3B0}"/>
+    <hyperlink ref="E8" r:id="rId56" xr:uid="{1A110A73-AF6F-42C2-ABF9-AAE664D5C803}"/>
+    <hyperlink ref="E11" r:id="rId57" xr:uid="{AEF75919-FFA5-4EFB-8F0C-DD6EA97C52D0}"/>
+    <hyperlink ref="F11" r:id="rId58" xr:uid="{6D4C7E16-1F1F-457D-9CE7-B6F036D16092}"/>
+    <hyperlink ref="F49" r:id="rId59" xr:uid="{6D16B745-748A-4C03-AE23-93A3278F3011}"/>
+    <hyperlink ref="F8" r:id="rId60" xr:uid="{54B0060D-FB7B-4C27-A4F4-D7D163F07D32}"/>
+    <hyperlink ref="F4" r:id="rId61" location=":~:text=Teaching%20Kids%20to%20Cope%20%28TKC%29%201%20About%20This,Training%20...%205%20Relevant%20Published%2C%20Peer-Reviewed%20Research%20" xr:uid="{006908E9-8A98-4D4A-83B1-FDF2CE103984}"/>
+    <hyperlink ref="F61" r:id="rId62" xr:uid="{396A14E9-844B-4BE0-A2DD-DB79A40B6B7D}"/>
+    <hyperlink ref="E61" r:id="rId63" xr:uid="{97C70E8E-3BD4-4E36-9080-331B9BB33B82}"/>
+    <hyperlink ref="E17" r:id="rId64" xr:uid="{850EDBD9-B7CE-4676-A30A-402D87A16189}"/>
+    <hyperlink ref="E53" r:id="rId65" xr:uid="{D3F7048B-8C03-4357-B3E3-98E7E9582490}"/>
+    <hyperlink ref="E28" r:id="rId66" xr:uid="{6D7E6002-0EC7-4E95-B9F1-FC35174A9A74}"/>
+    <hyperlink ref="E4" r:id="rId67" xr:uid="{A5C7D15C-F513-476B-BD7F-801E08AE14FB}"/>
+    <hyperlink ref="E44" r:id="rId68" xr:uid="{EB393916-1222-4C26-A520-5AE7CE7C3FC8}"/>
+    <hyperlink ref="E12" r:id="rId69" xr:uid="{293BE39E-26D2-4702-AC75-39925DFFB037}"/>
+    <hyperlink ref="E51" r:id="rId70" xr:uid="{CD3D3293-A4E7-4BF7-8BF5-902A73911E06}"/>
+    <hyperlink ref="E47" r:id="rId71" xr:uid="{BBE6FAA5-503C-4552-9174-925C95799E9E}"/>
+    <hyperlink ref="E3" r:id="rId72" xr:uid="{380AFDDB-BEC4-42BA-9386-8CE1660523EF}"/>
+    <hyperlink ref="F3" r:id="rId73" xr:uid="{2DC27288-9647-4A2F-930E-A7B35AA9B75A}"/>
+    <hyperlink ref="E2" r:id="rId74" xr:uid="{96690CF7-D06C-49BE-83AB-DF5E462020C1}"/>
+    <hyperlink ref="E46" r:id="rId75" xr:uid="{219720DE-D671-48C6-BD3A-8CE209F35E0A}"/>
+    <hyperlink ref="E58" r:id="rId76" xr:uid="{20AFB83C-828D-4D3F-B126-3DD53FA97F3F}"/>
+    <hyperlink ref="F37" r:id="rId77" xr:uid="{DD12564D-BB5D-4101-B15A-06B8054CD078}"/>
+    <hyperlink ref="E37" r:id="rId78" xr:uid="{E497110D-04BE-43DD-8039-BC3F013C7251}"/>
+    <hyperlink ref="E41" r:id="rId79" xr:uid="{E46D299F-3A2E-4D0F-B573-848E0D235B83}"/>
+    <hyperlink ref="E38" r:id="rId80" xr:uid="{BCB98A1A-A75D-4D44-801D-3DC91C576855}"/>
+    <hyperlink ref="F54" r:id="rId81" xr:uid="{7FD3E557-1A72-480C-87BE-7B9C5C289B24}"/>
+    <hyperlink ref="E54" r:id="rId82" xr:uid="{12E4E088-F11C-47A2-A449-08D5D80D923B}"/>
+    <hyperlink ref="E48" r:id="rId83" xr:uid="{35EE0DAA-3514-4409-A76C-FB785AB3084C}"/>
+    <hyperlink ref="E52" r:id="rId84" xr:uid="{F66EB814-4D6B-46D8-BEDD-4C5ED487B5A8}"/>
+    <hyperlink ref="F46" r:id="rId85" xr:uid="{CD36F694-38EB-4358-9D90-D0939030C765}"/>
+    <hyperlink ref="F58" r:id="rId86" xr:uid="{99B79EA3-F4BF-4D3E-8A9B-507BF653B0F4}"/>
+    <hyperlink ref="F28" r:id="rId87" xr:uid="{01575AEF-E417-4E1B-A302-19D757A77FB0}"/>
+    <hyperlink ref="F6" r:id="rId88" xr:uid="{4A83D453-C35E-482B-B244-FFF25A75ADB7}"/>
+    <hyperlink ref="E6" r:id="rId89" xr:uid="{E5B72362-341D-4F57-BB43-79649F216DF6}"/>
+    <hyperlink ref="F13" r:id="rId90" xr:uid="{1DB53E18-BBC5-4004-9416-A89A0CEE612F}"/>
+    <hyperlink ref="F18" r:id="rId91" xr:uid="{AD6D22EF-27CC-4C5B-A487-4DFA98DC121B}"/>
+    <hyperlink ref="F25" r:id="rId92" xr:uid="{94CDFDD0-5AB5-4631-B9A8-F1E850421907}"/>
+    <hyperlink ref="E25" r:id="rId93" xr:uid="{DF210E38-396F-49D9-8988-EA0C097A4BB8}"/>
+    <hyperlink ref="F36" r:id="rId94" xr:uid="{3FC495AD-261C-431B-BD91-B6AD52C5A642}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Intervention filter to dashboard
</commit_message>
<xml_diff>
--- a/data/DPO_app_intervention_names.xlsx
+++ b/data/DPO_app_intervention_names.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoregon-my.sharepoint.com/personal/strevino_uoregon_edu/Documents/Desktop/HEDCO Institute/GitHub R Projects/Depression_Prevention_Overview/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="8_{8A08B8BF-4197-4250-9F47-B55103264D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17566173-E6ED-43FB-8978-4891535000E9}"/>
+  <xr:revisionPtr revIDLastSave="308" documentId="8_{8A08B8BF-4197-4250-9F47-B55103264D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99966BC9-5E79-4797-9E12-46F442B71CEB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{ECE45DD1-0422-437C-B3F3-CDDA7BE602A8}"/>
+    <workbookView xWindow="28680" yWindow="-255" windowWidth="16440" windowHeight="28320" xr2:uid="{ECE45DD1-0422-437C-B3F3-CDDA7BE602A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Rename" sheetId="1" r:id="rId1"/>
     <sheet name="Definitions" sheetId="2" r:id="rId2"/>
     <sheet name="Links" sheetId="3" r:id="rId3"/>
+    <sheet name="Intervention filters" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Links!$A$1:$D$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Links!$A$1:$F$64</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Rename!$C$1:$F$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="255">
   <si>
     <t>Intervention</t>
   </si>
@@ -740,9 +741,6 @@
     <t>The Optimism and Life Skills Program (adapted from Penn Depression Prevention Program)</t>
   </si>
   <si>
-    <t>Cognitive-behavior program (CB; adapted); interpersonal psychotherapy–adolescent skills training (IPT-AST)</t>
-  </si>
-  <si>
     <t>https://research.kpchr.org/Research/Research-Areas/Mental-Health/Youth-Depression-Programs#Downloads</t>
   </si>
   <si>
@@ -753,13 +751,73 @@
   </si>
   <si>
     <t>https://guidebook.eif.org.uk/programme/penn-resilience-programme-uk-implementation-in-primary-school</t>
+  </si>
+  <si>
+    <t>Emotion regulation program; Behavioral activation program</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Dot be</t>
+  </si>
+  <si>
+    <t>SPARX</t>
+  </si>
+  <si>
+    <t>Adolescents Coping with Emotions</t>
+  </si>
+  <si>
+    <t>Girls in Transition</t>
+  </si>
+  <si>
+    <t>Unified Protocol for Transdiagnostic Treatment of Emotional Disorders in Adolescents</t>
+  </si>
+  <si>
+    <t>Beyondblue</t>
+  </si>
+  <si>
+    <t>Cognitive Behavioral Programs</t>
+  </si>
+  <si>
+    <t>Control, Responsibility, Awareness, Impetus, and Confidence</t>
+  </si>
+  <si>
+    <t>Interpersonal Psychotherapy-Adolescent Skills Training</t>
+  </si>
+  <si>
+    <t>Cognitive-behavior program (CB; adapted); Interpersonal Psychotherapy–Adolescent Skills Training (IPT-AST)</t>
+  </si>
+  <si>
+    <t>Thiswayup</t>
+  </si>
+  <si>
+    <t>Emotion Regulation Programs</t>
+  </si>
+  <si>
+    <t>Behavioral Activation Programs</t>
+  </si>
+  <si>
+    <t>Other Prevention Program</t>
+  </si>
+  <si>
+    <t>Peer Interaction</t>
+  </si>
+  <si>
+    <t>Social Skills Training</t>
+  </si>
+  <si>
+    <t>Psychoeducational Intervention</t>
+  </si>
+  <si>
+    <t>Cognitive-behavior group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -782,8 +840,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -793,6 +859,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -810,7 +888,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -821,15 +899,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1182,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09150482-75BD-4133-A06F-6CE7E7EB8102}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,6 +1715,9 @@
       <c r="C22" t="s">
         <v>3</v>
       </c>
+      <c r="D22" t="s">
+        <v>254</v>
+      </c>
       <c r="E22" t="s">
         <v>65</v>
       </c>
@@ -1695,6 +1792,9 @@
       <c r="C26" t="s">
         <v>2</v>
       </c>
+      <c r="D26" t="s">
+        <v>235</v>
+      </c>
       <c r="E26" t="s">
         <v>65</v>
       </c>
@@ -1951,7 +2051,7 @@
         <v>42</v>
       </c>
       <c r="D41" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="E41" t="s">
         <v>66</v>
@@ -2252,15 +2352,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>31859</v>
       </c>
       <c r="B59" t="s">
         <v>153</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="5" t="s">
         <v>51</v>
+      </c>
+      <c r="D59" t="s">
+        <v>174</v>
       </c>
       <c r="E59" t="s">
         <v>66</v>
@@ -2465,6 +2568,9 @@
       </c>
       <c r="C71" t="s">
         <v>13</v>
+      </c>
+      <c r="D71" t="s">
+        <v>245</v>
       </c>
       <c r="E71" t="s">
         <v>66</v>
@@ -2488,7 +2594,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,8 +2799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{504B7D24-44EE-4748-B674-AFAEE10AE69B}">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2728,702 +2834,698 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>31788</v>
+        <v>31883</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>171</v>
+      <c r="D2" t="s">
+        <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>31792</v>
+        <v>31881</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>31881</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>31835</v>
+      </c>
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>31807</v>
-      </c>
-      <c r="B4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>31809</v>
-      </c>
-      <c r="B5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>188</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>201</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>31809</v>
+        <v>31815</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>70</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>31809</v>
+        <v>32054</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>190</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>31815</v>
+        <v>31953</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>31816</v>
+        <v>31857</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>31818</v>
+        <v>31857</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>184</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>31835</v>
+        <v>31858</v>
       </c>
       <c r="B11" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>31882</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>31868</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>31853</v>
+      </c>
+      <c r="B14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>31885</v>
+      </c>
+      <c r="B15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>32232</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>31792</v>
+      </c>
+      <c r="B17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>31842</v>
-      </c>
-      <c r="B12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>31845</v>
-      </c>
-      <c r="B13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>31847</v>
-      </c>
-      <c r="B14" t="s">
-        <v>128</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>31848</v>
-      </c>
-      <c r="B15" t="s">
-        <v>155</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>31851</v>
-      </c>
-      <c r="B16" t="s">
-        <v>121</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>31853</v>
-      </c>
-      <c r="B17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F17" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>31855</v>
+        <v>31909</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>31857</v>
+        <v>32180</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>184</v>
+        <v>5</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>31857</v>
+        <v>32283</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>185</v>
+        <v>6</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>31858</v>
+        <v>31886</v>
       </c>
       <c r="B21" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>31859</v>
+        <v>31915</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>202</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>31860</v>
+        <v>31885</v>
       </c>
       <c r="B23" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>187</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>31863</v>
+        <v>32203</v>
       </c>
       <c r="B24" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>31865</v>
+        <v>31788</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>56</v>
+      <c r="D25" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>31867</v>
+        <v>31863</v>
       </c>
       <c r="B26" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>31868</v>
+        <v>31920</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
+        <v>167</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>15</v>
+      <c r="D27" t="s">
+        <v>31</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>31869</v>
+        <v>31958</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>31870</v>
+        <v>31867</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>174</v>
+      <c r="D29" t="s">
+        <v>48</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>31875</v>
+        <v>31904</v>
       </c>
       <c r="B30" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>178</v>
+      <c r="D30" t="s">
+        <v>39</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31">
+        <v>32265</v>
+      </c>
+      <c r="B31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32269</v>
+      </c>
+      <c r="B32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31845</v>
+      </c>
+      <c r="B33" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34">
         <v>31879</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" t="s">
         <v>119</v>
       </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31881</v>
-      </c>
-      <c r="B32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>182</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>31881</v>
-      </c>
-      <c r="B33" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>183</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>31882</v>
-      </c>
-      <c r="B34" t="s">
-        <v>118</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>31883</v>
+        <v>31809</v>
       </c>
       <c r="B35" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>188</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>31885</v>
+        <v>31809</v>
       </c>
       <c r="B36" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>186</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>31885</v>
+        <v>31870</v>
       </c>
       <c r="B37" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>187</v>
+        <v>1</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>31886</v>
+        <v>31859</v>
       </c>
       <c r="B38" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>216</v>
+        <v>201</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -3446,104 +3548,100 @@
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>31904</v>
+        <v>32316</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>31909</v>
+        <v>31855</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>219</v>
+        <v>229</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>31915</v>
+        <v>31818</v>
       </c>
       <c r="B42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>30</v>
-      </c>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>31920</v>
+        <v>31816</v>
       </c>
       <c r="B43" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>31</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>211</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>31947</v>
+        <v>31848</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>220</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>31950</v>
+        <v>31860</v>
       </c>
       <c r="B45" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>191</v>
+      <c r="D45" t="s">
+        <v>35</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>206</v>
@@ -3560,13 +3658,13 @@
         <v>159</v>
       </c>
       <c r="C46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>207</v>
@@ -3574,71 +3672,76 @@
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>31953</v>
+        <v>32238</v>
       </c>
       <c r="B47" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="D47" t="s">
-        <v>46</v>
+      <c r="D47" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="F47" s="4"/>
+        <v>206</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>31958</v>
+        <v>31950</v>
       </c>
       <c r="B48" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C48">
-        <v>1</v>
-      </c>
-      <c r="D48" t="s">
-        <v>58</v>
+        <v>2</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>32054</v>
+        <v>32238</v>
       </c>
       <c r="B49" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="C49">
-        <v>1</v>
-      </c>
-      <c r="D49" t="s">
-        <v>70</v>
+        <v>2</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>32067</v>
+        <v>31851</v>
       </c>
       <c r="B50" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>175</v>
+        <v>69</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>206</v>
@@ -3649,375 +3752,1764 @@
     </row>
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>32137</v>
+        <v>32067</v>
       </c>
       <c r="B51" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>64</v>
+        <v>175</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>224</v>
+        <v>206</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>32174</v>
+        <v>31847</v>
       </c>
       <c r="B52" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>234</v>
+        <v>71</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>32180</v>
+        <v>32320</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="C53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>225</v>
+        <v>206</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>32203</v>
+        <v>32288</v>
       </c>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>31875</v>
+      </c>
+      <c r="B55" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>31809</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56">
         <v>2</v>
       </c>
-      <c r="D54" t="s">
-        <v>13</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>32232</v>
-      </c>
-      <c r="B55" t="s">
-        <v>124</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>32233</v>
-      </c>
-      <c r="B56" t="s">
-        <v>115</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
       <c r="D56" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" s="4"/>
+        <v>189</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>32238</v>
+        <v>31869</v>
       </c>
       <c r="B57" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
-      <c r="D57" s="1" t="s">
-        <v>191</v>
+      <c r="D57" t="s">
+        <v>11</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>32238</v>
+        <v>31807</v>
       </c>
       <c r="B58" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="C58">
-        <v>2</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>192</v>
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>50</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>221</v>
+        <v>199</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>32265</v>
+        <v>31947</v>
       </c>
       <c r="B59" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>32269</v>
+        <v>31865</v>
       </c>
       <c r="B60" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
-      <c r="D60" t="s">
-        <v>39</v>
+      <c r="D60" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>32283</v>
+        <v>31842</v>
       </c>
       <c r="B61" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>32288</v>
+        <v>32233</v>
       </c>
       <c r="B62" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C62">
         <v>1</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>32316</v>
+        <v>32174</v>
       </c>
       <c r="B63" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="C63">
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>41</v>
+        <v>233</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>201</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>32320</v>
+        <v>32137</v>
       </c>
       <c r="B64" t="s">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D65" xr:uid="{504B7D24-44EE-4748-B674-AFAEE10AE69B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D65">
-      <sortCondition ref="B1:B65"/>
+  <autoFilter ref="A1:F64" xr:uid="{504B7D24-44EE-4748-B674-AFAEE10AE69B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F64">
+      <sortCondition ref="D1:D64"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
     <sortCondition ref="A2:A64"/>
   </sortState>
   <conditionalFormatting sqref="B1:C1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F45" r:id="rId1" xr:uid="{8378A75F-103E-494E-BCD6-7E8B0FC2607A}"/>
-    <hyperlink ref="F57" r:id="rId2" xr:uid="{1EF98329-AD6E-4032-A1E0-D712A8F13790}"/>
-    <hyperlink ref="F50" r:id="rId3" xr:uid="{17F69C15-BC09-4D1C-ACD2-30F2650F42D3}"/>
-    <hyperlink ref="F62" r:id="rId4" xr:uid="{BAFE6581-8387-44F8-9581-6056EF67AD2B}"/>
-    <hyperlink ref="F30" r:id="rId5" xr:uid="{4681AFB0-1100-4894-B106-BAB05E220DC9}"/>
-    <hyperlink ref="F23" r:id="rId6" xr:uid="{0E1741F3-B332-472E-93EE-30490FD72656}"/>
-    <hyperlink ref="F16" r:id="rId7" xr:uid="{B2BE18D4-8FFF-4DCA-A8E7-29C6070FDC14}"/>
-    <hyperlink ref="F14" r:id="rId8" xr:uid="{06DC273A-1AA0-49F3-96C2-1B38917EE67A}"/>
-    <hyperlink ref="F64" r:id="rId9" xr:uid="{071B8E4E-EF55-41B5-B9CA-5C50C5ED8A33}"/>
+    <hyperlink ref="F46" r:id="rId1" xr:uid="{8378A75F-103E-494E-BCD6-7E8B0FC2607A}"/>
+    <hyperlink ref="F47" r:id="rId2" xr:uid="{1EF98329-AD6E-4032-A1E0-D712A8F13790}"/>
+    <hyperlink ref="F51" r:id="rId3" xr:uid="{17F69C15-BC09-4D1C-ACD2-30F2650F42D3}"/>
+    <hyperlink ref="F54" r:id="rId4" xr:uid="{BAFE6581-8387-44F8-9581-6056EF67AD2B}"/>
+    <hyperlink ref="F55" r:id="rId5" xr:uid="{4681AFB0-1100-4894-B106-BAB05E220DC9}"/>
+    <hyperlink ref="F45" r:id="rId6" xr:uid="{0E1741F3-B332-472E-93EE-30490FD72656}"/>
+    <hyperlink ref="F50" r:id="rId7" xr:uid="{B2BE18D4-8FFF-4DCA-A8E7-29C6070FDC14}"/>
+    <hyperlink ref="F52" r:id="rId8" xr:uid="{06DC273A-1AA0-49F3-96C2-1B38917EE67A}"/>
+    <hyperlink ref="F53" r:id="rId9" xr:uid="{071B8E4E-EF55-41B5-B9CA-5C50C5ED8A33}"/>
     <hyperlink ref="F39" r:id="rId10" xr:uid="{ECE55C7D-5F7C-4CD6-AE7B-BB776B91FEC0}"/>
-    <hyperlink ref="F63" r:id="rId11" xr:uid="{F528B45E-8A70-4F2B-9B56-34EA1D177F91}"/>
-    <hyperlink ref="F29" r:id="rId12" xr:uid="{9F8E7070-E516-4E38-8727-D35DDAF3AAFA}"/>
-    <hyperlink ref="F5" r:id="rId13" xr:uid="{4C671029-11A2-42D4-90B6-FE8A2F496E66}"/>
-    <hyperlink ref="F34" r:id="rId14" xr:uid="{6E7B255F-A1E6-47AD-AF0E-0E0134578ACE}"/>
-    <hyperlink ref="F21" r:id="rId15" xr:uid="{AF042E5E-FAFF-454F-876A-99CC8A53F2D8}"/>
-    <hyperlink ref="F27" r:id="rId16" xr:uid="{5FCE0664-D7B0-41A6-90BA-460A778BBD4E}"/>
-    <hyperlink ref="F19" r:id="rId17" xr:uid="{E907D68D-C888-4FC2-A814-F8543EAE33BA}"/>
-    <hyperlink ref="F20" r:id="rId18" xr:uid="{0D2AFB46-6043-43B0-91B3-3016DD2F06D8}"/>
-    <hyperlink ref="E23" r:id="rId19" xr:uid="{F7EA67C3-4E5A-4E4A-BAC7-814EDDD6604F}"/>
-    <hyperlink ref="E45" r:id="rId20" xr:uid="{E211FF3E-8ACA-4D6F-9E5D-DFE9755EF792}"/>
-    <hyperlink ref="E57" r:id="rId21" xr:uid="{01A2681D-B4A1-4CA1-94E5-12FAEAB52794}"/>
-    <hyperlink ref="E16" r:id="rId22" xr:uid="{B0917317-6B73-48E2-8AC8-1820D1B7E9F0}"/>
-    <hyperlink ref="E50" r:id="rId23" xr:uid="{0188ED8A-3E1A-4320-BE5A-F1FC88B927CC}"/>
-    <hyperlink ref="E14" r:id="rId24" xr:uid="{5AD57216-123A-4604-BA8C-514093EC5656}"/>
-    <hyperlink ref="E64" r:id="rId25" xr:uid="{3A07E0DC-5F13-4DBB-B768-03A3683F2F2B}"/>
-    <hyperlink ref="E62" r:id="rId26" xr:uid="{D7BB18F4-8F0E-4144-A0EF-19C7CDD337CC}"/>
-    <hyperlink ref="E30" r:id="rId27" xr:uid="{113F81A6-9FBE-4EF0-BF55-D14AD78DC90F}"/>
-    <hyperlink ref="E29" r:id="rId28" xr:uid="{881201B8-A3DC-44FF-AF57-F959E27D70B4}"/>
-    <hyperlink ref="E22" r:id="rId29" xr:uid="{74D36768-F7E8-4844-99A6-F07AECA72B32}"/>
+    <hyperlink ref="F40" r:id="rId11" xr:uid="{F528B45E-8A70-4F2B-9B56-34EA1D177F91}"/>
+    <hyperlink ref="F37" r:id="rId12" xr:uid="{9F8E7070-E516-4E38-8727-D35DDAF3AAFA}"/>
+    <hyperlink ref="F35" r:id="rId13" xr:uid="{4C671029-11A2-42D4-90B6-FE8A2F496E66}"/>
+    <hyperlink ref="F12" r:id="rId14" xr:uid="{6E7B255F-A1E6-47AD-AF0E-0E0134578ACE}"/>
+    <hyperlink ref="F11" r:id="rId15" xr:uid="{AF042E5E-FAFF-454F-876A-99CC8A53F2D8}"/>
+    <hyperlink ref="F13" r:id="rId16" xr:uid="{5FCE0664-D7B0-41A6-90BA-460A778BBD4E}"/>
+    <hyperlink ref="F10" r:id="rId17" xr:uid="{E907D68D-C888-4FC2-A814-F8543EAE33BA}"/>
+    <hyperlink ref="F9" r:id="rId18" xr:uid="{0D2AFB46-6043-43B0-91B3-3016DD2F06D8}"/>
+    <hyperlink ref="E45" r:id="rId19" xr:uid="{F7EA67C3-4E5A-4E4A-BAC7-814EDDD6604F}"/>
+    <hyperlink ref="E46" r:id="rId20" xr:uid="{E211FF3E-8ACA-4D6F-9E5D-DFE9755EF792}"/>
+    <hyperlink ref="E47" r:id="rId21" xr:uid="{01A2681D-B4A1-4CA1-94E5-12FAEAB52794}"/>
+    <hyperlink ref="E50" r:id="rId22" xr:uid="{B0917317-6B73-48E2-8AC8-1820D1B7E9F0}"/>
+    <hyperlink ref="E51" r:id="rId23" xr:uid="{0188ED8A-3E1A-4320-BE5A-F1FC88B927CC}"/>
+    <hyperlink ref="E52" r:id="rId24" xr:uid="{5AD57216-123A-4604-BA8C-514093EC5656}"/>
+    <hyperlink ref="E53" r:id="rId25" xr:uid="{3A07E0DC-5F13-4DBB-B768-03A3683F2F2B}"/>
+    <hyperlink ref="E54" r:id="rId26" xr:uid="{D7BB18F4-8F0E-4144-A0EF-19C7CDD337CC}"/>
+    <hyperlink ref="E55" r:id="rId27" xr:uid="{113F81A6-9FBE-4EF0-BF55-D14AD78DC90F}"/>
+    <hyperlink ref="E37" r:id="rId28" xr:uid="{881201B8-A3DC-44FF-AF57-F959E27D70B4}"/>
+    <hyperlink ref="E38" r:id="rId29" xr:uid="{74D36768-F7E8-4844-99A6-F07AECA72B32}"/>
     <hyperlink ref="E39" r:id="rId30" xr:uid="{A13FF7A5-9F91-4F1A-8B36-38D83EBA4CF6}"/>
-    <hyperlink ref="E63" r:id="rId31" xr:uid="{F832A250-EF1C-43A1-B152-5FAC9AD93157}"/>
-    <hyperlink ref="E13" r:id="rId32" xr:uid="{20AF2881-6D13-4C13-9979-EC975005CFB4}"/>
-    <hyperlink ref="E31" r:id="rId33" xr:uid="{0CB9A7E8-C383-4B63-ACAE-18F513DC04BA}"/>
-    <hyperlink ref="E5" r:id="rId34" xr:uid="{F1FFB753-1476-4A4E-85B6-FB513D590226}"/>
-    <hyperlink ref="E20" r:id="rId35" xr:uid="{E9771604-DF3A-43B7-A7DB-E53876A949F9}"/>
-    <hyperlink ref="E19" r:id="rId36" xr:uid="{4A162E7F-061C-4A0C-A88B-8FD04AB15516}"/>
-    <hyperlink ref="E34" r:id="rId37" xr:uid="{BA8288E1-5257-44C8-A76C-AD2147C98CA6}"/>
-    <hyperlink ref="E21" r:id="rId38" xr:uid="{8752A4AB-09BC-4D5E-8CF3-94D69B96AC52}"/>
-    <hyperlink ref="E27" r:id="rId39" xr:uid="{6620F9ED-DF56-402D-AB42-71003A0D8EA4}"/>
-    <hyperlink ref="E43" r:id="rId40" xr:uid="{5B949B19-D0A2-49FD-8D74-A9D7987E97A8}"/>
-    <hyperlink ref="E24" r:id="rId41" xr:uid="{DDDA1C3D-CB6F-4A49-8123-0F1377530EFC}"/>
-    <hyperlink ref="E26" r:id="rId42" xr:uid="{BF859DE6-C972-40AC-876E-6A05A58DEDB3}"/>
-    <hyperlink ref="E40" r:id="rId43" xr:uid="{859D5689-2AFC-47D9-9CDA-A1D5E95D534D}"/>
-    <hyperlink ref="E60" r:id="rId44" xr:uid="{DA936187-D053-4EA4-800E-AA1C70DFC567}"/>
-    <hyperlink ref="E59" r:id="rId45" xr:uid="{2B63FB07-176A-497B-B8A7-F76B009DC435}"/>
-    <hyperlink ref="F40" r:id="rId46" xr:uid="{66144401-076B-4D65-9B27-0F62CD92215C}"/>
-    <hyperlink ref="F60" r:id="rId47" xr:uid="{C9DB3F47-D825-4972-8C6F-6937F50DF437}"/>
-    <hyperlink ref="F59" r:id="rId48" xr:uid="{554860CA-220F-45D1-879B-A791B2E88D8C}"/>
-    <hyperlink ref="E35" r:id="rId49" xr:uid="{3F575516-1D65-4892-920A-97F6439B631E}"/>
-    <hyperlink ref="E33" r:id="rId50" xr:uid="{7A6C9AF8-5CCE-4A70-9BDF-A7383AA9FB4E}"/>
-    <hyperlink ref="E32" r:id="rId51" xr:uid="{744DE233-DC04-4235-907E-64E5F19A23BC}"/>
-    <hyperlink ref="F35" r:id="rId52" xr:uid="{B20D6884-6865-4E1E-9E88-247DF5EF294E}"/>
-    <hyperlink ref="F33" r:id="rId53" xr:uid="{3112B712-3917-4CB6-9414-FB164FC2940A}"/>
-    <hyperlink ref="F32" r:id="rId54" xr:uid="{AA037FD7-70D4-42E3-9D2E-AC7BC4A77AE1}"/>
-    <hyperlink ref="E49" r:id="rId55" xr:uid="{E4FA4305-BC77-40FB-9B4C-0AE98E9FE3B0}"/>
-    <hyperlink ref="E8" r:id="rId56" xr:uid="{1A110A73-AF6F-42C2-ABF9-AAE664D5C803}"/>
-    <hyperlink ref="E11" r:id="rId57" xr:uid="{AEF75919-FFA5-4EFB-8F0C-DD6EA97C52D0}"/>
-    <hyperlink ref="F11" r:id="rId58" xr:uid="{6D4C7E16-1F1F-457D-9CE7-B6F036D16092}"/>
-    <hyperlink ref="F49" r:id="rId59" xr:uid="{6D16B745-748A-4C03-AE23-93A3278F3011}"/>
-    <hyperlink ref="F8" r:id="rId60" xr:uid="{54B0060D-FB7B-4C27-A4F4-D7D163F07D32}"/>
-    <hyperlink ref="F4" r:id="rId61" location=":~:text=Teaching%20Kids%20to%20Cope%20%28TKC%29%201%20About%20This,Training%20...%205%20Relevant%20Published%2C%20Peer-Reviewed%20Research%20" xr:uid="{006908E9-8A98-4D4A-83B1-FDF2CE103984}"/>
-    <hyperlink ref="F61" r:id="rId62" xr:uid="{396A14E9-844B-4BE0-A2DD-DB79A40B6B7D}"/>
-    <hyperlink ref="E61" r:id="rId63" xr:uid="{97C70E8E-3BD4-4E36-9080-331B9BB33B82}"/>
-    <hyperlink ref="E17" r:id="rId64" xr:uid="{850EDBD9-B7CE-4676-A30A-402D87A16189}"/>
-    <hyperlink ref="E53" r:id="rId65" xr:uid="{D3F7048B-8C03-4357-B3E3-98E7E9582490}"/>
-    <hyperlink ref="E28" r:id="rId66" xr:uid="{6D7E6002-0EC7-4E95-B9F1-FC35174A9A74}"/>
-    <hyperlink ref="E4" r:id="rId67" xr:uid="{A5C7D15C-F513-476B-BD7F-801E08AE14FB}"/>
-    <hyperlink ref="E44" r:id="rId68" xr:uid="{EB393916-1222-4C26-A520-5AE7CE7C3FC8}"/>
-    <hyperlink ref="E12" r:id="rId69" xr:uid="{293BE39E-26D2-4702-AC75-39925DFFB037}"/>
-    <hyperlink ref="E51" r:id="rId70" xr:uid="{CD3D3293-A4E7-4BF7-8BF5-902A73911E06}"/>
-    <hyperlink ref="E47" r:id="rId71" xr:uid="{BBE6FAA5-503C-4552-9174-925C95799E9E}"/>
-    <hyperlink ref="E3" r:id="rId72" xr:uid="{380AFDDB-BEC4-42BA-9386-8CE1660523EF}"/>
-    <hyperlink ref="F3" r:id="rId73" xr:uid="{2DC27288-9647-4A2F-930E-A7B35AA9B75A}"/>
-    <hyperlink ref="E2" r:id="rId74" xr:uid="{96690CF7-D06C-49BE-83AB-DF5E462020C1}"/>
-    <hyperlink ref="E46" r:id="rId75" xr:uid="{219720DE-D671-48C6-BD3A-8CE209F35E0A}"/>
-    <hyperlink ref="E58" r:id="rId76" xr:uid="{20AFB83C-828D-4D3F-B126-3DD53FA97F3F}"/>
-    <hyperlink ref="F37" r:id="rId77" xr:uid="{DD12564D-BB5D-4101-B15A-06B8054CD078}"/>
-    <hyperlink ref="E37" r:id="rId78" xr:uid="{E497110D-04BE-43DD-8039-BC3F013C7251}"/>
-    <hyperlink ref="E41" r:id="rId79" xr:uid="{E46D299F-3A2E-4D0F-B573-848E0D235B83}"/>
-    <hyperlink ref="E38" r:id="rId80" xr:uid="{BCB98A1A-A75D-4D44-801D-3DC91C576855}"/>
-    <hyperlink ref="F54" r:id="rId81" xr:uid="{7FD3E557-1A72-480C-87BE-7B9C5C289B24}"/>
-    <hyperlink ref="E54" r:id="rId82" xr:uid="{12E4E088-F11C-47A2-A449-08D5D80D923B}"/>
-    <hyperlink ref="E48" r:id="rId83" xr:uid="{35EE0DAA-3514-4409-A76C-FB785AB3084C}"/>
-    <hyperlink ref="E52" r:id="rId84" xr:uid="{F66EB814-4D6B-46D8-BEDD-4C5ED487B5A8}"/>
-    <hyperlink ref="F46" r:id="rId85" xr:uid="{CD36F694-38EB-4358-9D90-D0939030C765}"/>
-    <hyperlink ref="F58" r:id="rId86" xr:uid="{99B79EA3-F4BF-4D3E-8A9B-507BF653B0F4}"/>
-    <hyperlink ref="F28" r:id="rId87" xr:uid="{01575AEF-E417-4E1B-A302-19D757A77FB0}"/>
-    <hyperlink ref="F6" r:id="rId88" xr:uid="{4A83D453-C35E-482B-B244-FFF25A75ADB7}"/>
-    <hyperlink ref="E6" r:id="rId89" xr:uid="{E5B72362-341D-4F57-BB43-79649F216DF6}"/>
-    <hyperlink ref="F13" r:id="rId90" xr:uid="{1DB53E18-BBC5-4004-9416-A89A0CEE612F}"/>
-    <hyperlink ref="F18" r:id="rId91" xr:uid="{AD6D22EF-27CC-4C5B-A487-4DFA98DC121B}"/>
-    <hyperlink ref="F25" r:id="rId92" xr:uid="{94CDFDD0-5AB5-4631-B9A8-F1E850421907}"/>
-    <hyperlink ref="E25" r:id="rId93" xr:uid="{DF210E38-396F-49D9-8988-EA0C097A4BB8}"/>
-    <hyperlink ref="F36" r:id="rId94" xr:uid="{3FC495AD-261C-431B-BD91-B6AD52C5A642}"/>
+    <hyperlink ref="E40" r:id="rId31" xr:uid="{F832A250-EF1C-43A1-B152-5FAC9AD93157}"/>
+    <hyperlink ref="E33" r:id="rId32" xr:uid="{20AF2881-6D13-4C13-9979-EC975005CFB4}"/>
+    <hyperlink ref="E34" r:id="rId33" xr:uid="{0CB9A7E8-C383-4B63-ACAE-18F513DC04BA}"/>
+    <hyperlink ref="E35" r:id="rId34" xr:uid="{F1FFB753-1476-4A4E-85B6-FB513D590226}"/>
+    <hyperlink ref="E9" r:id="rId35" xr:uid="{E9771604-DF3A-43B7-A7DB-E53876A949F9}"/>
+    <hyperlink ref="E10" r:id="rId36" xr:uid="{4A162E7F-061C-4A0C-A88B-8FD04AB15516}"/>
+    <hyperlink ref="E12" r:id="rId37" xr:uid="{BA8288E1-5257-44C8-A76C-AD2147C98CA6}"/>
+    <hyperlink ref="E11" r:id="rId38" xr:uid="{8752A4AB-09BC-4D5E-8CF3-94D69B96AC52}"/>
+    <hyperlink ref="E13" r:id="rId39" xr:uid="{6620F9ED-DF56-402D-AB42-71003A0D8EA4}"/>
+    <hyperlink ref="E27" r:id="rId40" xr:uid="{5B949B19-D0A2-49FD-8D74-A9D7987E97A8}"/>
+    <hyperlink ref="E26" r:id="rId41" xr:uid="{DDDA1C3D-CB6F-4A49-8123-0F1377530EFC}"/>
+    <hyperlink ref="E29" r:id="rId42" xr:uid="{BF859DE6-C972-40AC-876E-6A05A58DEDB3}"/>
+    <hyperlink ref="E30" r:id="rId43" xr:uid="{859D5689-2AFC-47D9-9CDA-A1D5E95D534D}"/>
+    <hyperlink ref="E32" r:id="rId44" xr:uid="{DA936187-D053-4EA4-800E-AA1C70DFC567}"/>
+    <hyperlink ref="E31" r:id="rId45" xr:uid="{2B63FB07-176A-497B-B8A7-F76B009DC435}"/>
+    <hyperlink ref="F30" r:id="rId46" xr:uid="{66144401-076B-4D65-9B27-0F62CD92215C}"/>
+    <hyperlink ref="F32" r:id="rId47" xr:uid="{C9DB3F47-D825-4972-8C6F-6937F50DF437}"/>
+    <hyperlink ref="F31" r:id="rId48" xr:uid="{554860CA-220F-45D1-879B-A791B2E88D8C}"/>
+    <hyperlink ref="E2" r:id="rId49" xr:uid="{3F575516-1D65-4892-920A-97F6439B631E}"/>
+    <hyperlink ref="E3" r:id="rId50" xr:uid="{7A6C9AF8-5CCE-4A70-9BDF-A7383AA9FB4E}"/>
+    <hyperlink ref="E4" r:id="rId51" xr:uid="{744DE233-DC04-4235-907E-64E5F19A23BC}"/>
+    <hyperlink ref="F2" r:id="rId52" xr:uid="{B20D6884-6865-4E1E-9E88-247DF5EF294E}"/>
+    <hyperlink ref="F3" r:id="rId53" xr:uid="{3112B712-3917-4CB6-9414-FB164FC2940A}"/>
+    <hyperlink ref="F4" r:id="rId54" xr:uid="{AA037FD7-70D4-42E3-9D2E-AC7BC4A77AE1}"/>
+    <hyperlink ref="E7" r:id="rId55" xr:uid="{E4FA4305-BC77-40FB-9B4C-0AE98E9FE3B0}"/>
+    <hyperlink ref="E6" r:id="rId56" xr:uid="{1A110A73-AF6F-42C2-ABF9-AAE664D5C803}"/>
+    <hyperlink ref="E5" r:id="rId57" xr:uid="{AEF75919-FFA5-4EFB-8F0C-DD6EA97C52D0}"/>
+    <hyperlink ref="F5" r:id="rId58" xr:uid="{6D4C7E16-1F1F-457D-9CE7-B6F036D16092}"/>
+    <hyperlink ref="F7" r:id="rId59" xr:uid="{6D16B745-748A-4C03-AE23-93A3278F3011}"/>
+    <hyperlink ref="F6" r:id="rId60" xr:uid="{54B0060D-FB7B-4C27-A4F4-D7D163F07D32}"/>
+    <hyperlink ref="F58" r:id="rId61" location=":~:text=Teaching%20Kids%20to%20Cope%20%28TKC%29%201%20About%20This,Training%20...%205%20Relevant%20Published%2C%20Peer-Reviewed%20Research%20" xr:uid="{006908E9-8A98-4D4A-83B1-FDF2CE103984}"/>
+    <hyperlink ref="F20" r:id="rId62" xr:uid="{396A14E9-844B-4BE0-A2DD-DB79A40B6B7D}"/>
+    <hyperlink ref="E20" r:id="rId63" xr:uid="{97C70E8E-3BD4-4E36-9080-331B9BB33B82}"/>
+    <hyperlink ref="E14" r:id="rId64" xr:uid="{850EDBD9-B7CE-4676-A30A-402D87A16189}"/>
+    <hyperlink ref="E19" r:id="rId65" xr:uid="{D3F7048B-8C03-4357-B3E3-98E7E9582490}"/>
+    <hyperlink ref="E57" r:id="rId66" xr:uid="{6D7E6002-0EC7-4E95-B9F1-FC35174A9A74}"/>
+    <hyperlink ref="E58" r:id="rId67" xr:uid="{A5C7D15C-F513-476B-BD7F-801E08AE14FB}"/>
+    <hyperlink ref="E59" r:id="rId68" xr:uid="{EB393916-1222-4C26-A520-5AE7CE7C3FC8}"/>
+    <hyperlink ref="E61" r:id="rId69" xr:uid="{293BE39E-26D2-4702-AC75-39925DFFB037}"/>
+    <hyperlink ref="E64" r:id="rId70" xr:uid="{CD3D3293-A4E7-4BF7-8BF5-902A73911E06}"/>
+    <hyperlink ref="E8" r:id="rId71" xr:uid="{BBE6FAA5-503C-4552-9174-925C95799E9E}"/>
+    <hyperlink ref="E17" r:id="rId72" xr:uid="{380AFDDB-BEC4-42BA-9386-8CE1660523EF}"/>
+    <hyperlink ref="F17" r:id="rId73" xr:uid="{2DC27288-9647-4A2F-930E-A7B35AA9B75A}"/>
+    <hyperlink ref="E25" r:id="rId74" xr:uid="{96690CF7-D06C-49BE-83AB-DF5E462020C1}"/>
+    <hyperlink ref="E48" r:id="rId75" xr:uid="{219720DE-D671-48C6-BD3A-8CE209F35E0A}"/>
+    <hyperlink ref="E49" r:id="rId76" xr:uid="{20AFB83C-828D-4D3F-B126-3DD53FA97F3F}"/>
+    <hyperlink ref="F23" r:id="rId77" xr:uid="{DD12564D-BB5D-4101-B15A-06B8054CD078}"/>
+    <hyperlink ref="E23" r:id="rId78" xr:uid="{E497110D-04BE-43DD-8039-BC3F013C7251}"/>
+    <hyperlink ref="E18" r:id="rId79" xr:uid="{E46D299F-3A2E-4D0F-B573-848E0D235B83}"/>
+    <hyperlink ref="E21" r:id="rId80" xr:uid="{BCB98A1A-A75D-4D44-801D-3DC91C576855}"/>
+    <hyperlink ref="F24" r:id="rId81" xr:uid="{7FD3E557-1A72-480C-87BE-7B9C5C289B24}"/>
+    <hyperlink ref="E24" r:id="rId82" xr:uid="{12E4E088-F11C-47A2-A449-08D5D80D923B}"/>
+    <hyperlink ref="E28" r:id="rId83" xr:uid="{35EE0DAA-3514-4409-A76C-FB785AB3084C}"/>
+    <hyperlink ref="E63" r:id="rId84" xr:uid="{F66EB814-4D6B-46D8-BEDD-4C5ED487B5A8}"/>
+    <hyperlink ref="F48" r:id="rId85" xr:uid="{CD36F694-38EB-4358-9D90-D0939030C765}"/>
+    <hyperlink ref="F49" r:id="rId86" xr:uid="{99B79EA3-F4BF-4D3E-8A9B-507BF653B0F4}"/>
+    <hyperlink ref="F57" r:id="rId87" xr:uid="{01575AEF-E417-4E1B-A302-19D757A77FB0}"/>
+    <hyperlink ref="F56" r:id="rId88" xr:uid="{4A83D453-C35E-482B-B244-FFF25A75ADB7}"/>
+    <hyperlink ref="E56" r:id="rId89" xr:uid="{E5B72362-341D-4F57-BB43-79649F216DF6}"/>
+    <hyperlink ref="F33" r:id="rId90" xr:uid="{1DB53E18-BBC5-4004-9416-A89A0CEE612F}"/>
+    <hyperlink ref="F41" r:id="rId91" xr:uid="{AD6D22EF-27CC-4C5B-A487-4DFA98DC121B}"/>
+    <hyperlink ref="F60" r:id="rId92" xr:uid="{94CDFDD0-5AB5-4631-B9A8-F1E850421907}"/>
+    <hyperlink ref="E60" r:id="rId93" xr:uid="{DF210E38-396F-49D9-8988-EA0C097A4BB8}"/>
+    <hyperlink ref="F15" r:id="rId94" xr:uid="{3FC495AD-261C-431B-BD91-B6AD52C5A642}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{658FF64F-E427-49F5-95CD-E8023BDC665E}">
+  <dimension ref="A1:E80"/>
+  <sheetViews>
+    <sheetView topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="86" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>31883</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>31881</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>31881</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>31835</v>
+      </c>
+      <c r="B5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>31815</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>32054</v>
+      </c>
+      <c r="B7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>31953</v>
+      </c>
+      <c r="B8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>31857</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>31857</v>
+      </c>
+      <c r="B10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>31858</v>
+      </c>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>31882</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>31868</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>31853</v>
+      </c>
+      <c r="B14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>31885</v>
+      </c>
+      <c r="B15" t="s">
+        <v>143</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>32232</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>31792</v>
+      </c>
+      <c r="B17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>31909</v>
+      </c>
+      <c r="B18" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>32180</v>
+      </c>
+      <c r="B19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>32283</v>
+      </c>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>31886</v>
+      </c>
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>31915</v>
+      </c>
+      <c r="B22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>31885</v>
+      </c>
+      <c r="B23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>187</v>
+      </c>
+      <c r="E23" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>32203</v>
+      </c>
+      <c r="B24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>31788</v>
+      </c>
+      <c r="B25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E25" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>31863</v>
+      </c>
+      <c r="B26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>31920</v>
+      </c>
+      <c r="B27" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>31958</v>
+      </c>
+      <c r="B28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>31867</v>
+      </c>
+      <c r="B29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>31904</v>
+      </c>
+      <c r="B30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>32265</v>
+      </c>
+      <c r="B31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32269</v>
+      </c>
+      <c r="B32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31845</v>
+      </c>
+      <c r="B33" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31879</v>
+      </c>
+      <c r="B34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>31809</v>
+      </c>
+      <c r="B35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>188</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>31809</v>
+      </c>
+      <c r="B36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>31870</v>
+      </c>
+      <c r="B37" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E37" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>31859</v>
+      </c>
+      <c r="B38" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>31901</v>
+      </c>
+      <c r="B39" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>32316</v>
+      </c>
+      <c r="B40" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>31855</v>
+      </c>
+      <c r="B41" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>31818</v>
+      </c>
+      <c r="B42" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>31816</v>
+      </c>
+      <c r="B43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>31848</v>
+      </c>
+      <c r="B44" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+      <c r="E44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>31860</v>
+      </c>
+      <c r="B45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>31950</v>
+      </c>
+      <c r="B46" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>32238</v>
+      </c>
+      <c r="B47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>31950</v>
+      </c>
+      <c r="B48" t="s">
+        <v>159</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>32238</v>
+      </c>
+      <c r="B49" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>31851</v>
+      </c>
+      <c r="B50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>32067</v>
+      </c>
+      <c r="B51" t="s">
+        <v>151</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>175</v>
+      </c>
+      <c r="E51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>31847</v>
+      </c>
+      <c r="B52" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>71</v>
+      </c>
+      <c r="E52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>32320</v>
+      </c>
+      <c r="B53" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>71</v>
+      </c>
+      <c r="E53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>32288</v>
+      </c>
+      <c r="B54" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>31875</v>
+      </c>
+      <c r="B55" t="s">
+        <v>149</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>31809</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>189</v>
+      </c>
+      <c r="E56" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>31869</v>
+      </c>
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>31807</v>
+      </c>
+      <c r="B58" t="s">
+        <v>152</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>50</v>
+      </c>
+      <c r="E58" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>31947</v>
+      </c>
+      <c r="B59" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>31865</v>
+      </c>
+      <c r="B60" t="s">
+        <v>158</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>31842</v>
+      </c>
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>32233</v>
+      </c>
+      <c r="B62" t="s">
+        <v>115</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>32174</v>
+      </c>
+      <c r="B63" t="s">
+        <v>123</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>233</v>
+      </c>
+      <c r="E63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>32137</v>
+      </c>
+      <c r="B64" t="s">
+        <v>166</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>64</v>
+      </c>
+      <c r="E64" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>32120</v>
+      </c>
+      <c r="B65" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>85</v>
+      </c>
+      <c r="E65" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>32120</v>
+      </c>
+      <c r="B66" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>86</v>
+      </c>
+      <c r="E66" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>32096</v>
+      </c>
+      <c r="B67" t="s">
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>87</v>
+      </c>
+      <c r="E67" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>32175</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>31864</v>
+      </c>
+      <c r="B69" t="s">
+        <v>23</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E69" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>31840</v>
+      </c>
+      <c r="B70" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>88</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>31850</v>
+      </c>
+      <c r="B71" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s">
+        <v>89</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>31850</v>
+      </c>
+      <c r="B72" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72">
+        <v>3</v>
+      </c>
+      <c r="D72" t="s">
+        <v>90</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>31987</v>
+      </c>
+      <c r="B73" t="s">
+        <v>80</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>31987</v>
+      </c>
+      <c r="B74" t="s">
+        <v>79</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s">
+        <v>92</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>32172</v>
+      </c>
+      <c r="B75" t="s">
+        <v>60</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" t="s">
+        <v>93</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>31897</v>
+      </c>
+      <c r="B76" t="s">
+        <v>62</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>32016</v>
+      </c>
+      <c r="B77" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>94</v>
+      </c>
+      <c r="E77" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>31849</v>
+      </c>
+      <c r="B78" t="s">
+        <v>77</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78" t="s">
+        <v>95</v>
+      </c>
+      <c r="E78" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>31849</v>
+      </c>
+      <c r="B79" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>96</v>
+      </c>
+      <c r="E79" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>32255</v>
+      </c>
+      <c r="B80" t="s">
+        <v>59</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>97</v>
+      </c>
+      <c r="E80" t="s">
+        <v>253</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B81:C1048576 B1:C64 B65:B80 D65:D80 E65:E66 E70:E76 E78:E80">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix intervention filter and add Intervention summary statistic table (with temporary fix)
</commit_message>
<xml_diff>
--- a/data/DPO_app_intervention_names.xlsx
+++ b/data/DPO_app_intervention_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoregon-my.sharepoint.com/personal/strevino_uoregon_edu/Documents/Desktop/HEDCO Institute/GitHub R Projects/Depression_Prevention_Overview/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="308" documentId="8_{8A08B8BF-4197-4250-9F47-B55103264D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99966BC9-5E79-4797-9E12-46F442B71CEB}"/>
+  <xr:revisionPtr revIDLastSave="309" documentId="8_{8A08B8BF-4197-4250-9F47-B55103264D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C47C38A5-4C36-4321-BC30-5186E4E8170E}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-255" windowWidth="16440" windowHeight="28320" xr2:uid="{ECE45DD1-0422-437C-B3F3-CDDA7BE602A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ECE45DD1-0422-437C-B3F3-CDDA7BE602A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Rename" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="255">
   <si>
     <t>Intervention</t>
   </si>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09150482-75BD-4133-A06F-6CE7E7EB8102}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2500,6 +2500,9 @@
       </c>
       <c r="C67" t="s">
         <v>54</v>
+      </c>
+      <c r="D67" t="s">
+        <v>61</v>
       </c>
       <c r="E67" t="s">
         <v>66</v>

</xml_diff>